<commit_message>
[Pipette] 검토 data update
</commit_message>
<xml_diff>
--- a/Plasma_Pipette_PP Issue list.xlsx
+++ b/Plasma_Pipette_PP Issue list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEBEE13-4E52-47D9-A7C9-945907D84749}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FFBCB3-3BB8-45FE-B180-D26C67B04277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,14 +11,15 @@
     <sheet name="Issue" sheetId="1" r:id="rId1"/>
     <sheet name="1222 Meeting" sheetId="2" r:id="rId2"/>
     <sheet name="Sample" sheetId="3" r:id="rId3"/>
-    <sheet name="1225" sheetId="4" r:id="rId4"/>
+    <sheet name="Trans" sheetId="5" r:id="rId4"/>
+    <sheet name="1225" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="113">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,10 +50,6 @@
   </si>
   <si>
     <t>Trans 위치에 PCB cutting이 안되어 있음.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일단 Manual로 작업하고, PCB file에 V-Cut 표시 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -389,6 +386,99 @@
   <si>
     <t>Trans 2차측 GND는 1차측 GND에 연결되어야 함.
 -회로 수정 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 Manual로 작업하고, PCB file에 Board Cut out 표시 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V3.0 Battery Pack 사용 여부 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8V 외부에서 인가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4V 외부에서 인가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2차</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Layer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Turn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voltage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>측정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inductance-molding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M/E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trans molding case의 2차측 방향의 screw hole 위치가 전극과 가깝다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 조립시 비금속 제질의 screw 사용
+- 조립 hole를 GND PAD쪽으로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F/W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>완충 인식 안됨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -433,7 +523,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,8 +554,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -744,11 +840,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -765,12 +872,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -779,9 +880,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -856,37 +954,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -907,14 +978,66 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,6 +1059,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>40640</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BA77CD3-E380-4C55-B6B7-B4FFD78D72CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="711200" y="4168140"/>
+          <a:ext cx="6116320" cy="4587240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0134AA55-8665-482A-BA8D-2E3884E21C46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6967220" y="4160520"/>
+          <a:ext cx="6040120" cy="4530090"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1259,15 +1487,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:G20"/>
+  <dimension ref="B3:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
+    <col min="1" max="1" width="4.19921875" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.09765625" style="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
@@ -1294,213 +1522,381 @@
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B5" s="54">
+        <v>1</v>
+      </c>
+      <c r="C5" s="55">
+        <v>43456</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B6" s="38">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43456</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B5" s="41">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B7" s="38">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
         <v>43456</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F7" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B8" s="49">
+        <v>4</v>
+      </c>
+      <c r="C8" s="50">
+        <v>43456</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B9" s="49">
+        <v>5</v>
+      </c>
+      <c r="C9" s="50">
+        <v>43457</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B10" s="40">
+        <v>6</v>
+      </c>
+      <c r="C10" s="41">
+        <v>43458</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B11" s="40">
         <v>7</v>
       </c>
-      <c r="G5" s="62" t="s">
+      <c r="C11" s="41">
+        <v>43459</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="B12" s="40">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B6" s="42">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8">
-        <v>43456</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C12" s="41">
+        <v>43459</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B13" s="38">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6">
+        <v>43460</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B14" s="38">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6">
+        <v>43466</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B7" s="42">
+      <c r="E14" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B15" s="38">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43466</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8">
-        <v>43456</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="B8" s="42">
-        <v>4</v>
-      </c>
-      <c r="C8" s="8">
-        <v>43456</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="11" t="s">
+      <c r="E15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B16" s="38">
         <v>12</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B17" s="38">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B18" s="38">
         <v>14</v>
       </c>
-      <c r="G8" s="60" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="B9" s="42">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8">
-        <v>43457</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="61" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="B10" s="52">
-        <v>6</v>
-      </c>
-      <c r="C10" s="53">
-        <v>43458</v>
-      </c>
-      <c r="D10" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="B11" s="42">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8">
-        <v>43459</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="55" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="B12" s="42">
-        <v>8</v>
-      </c>
-      <c r="C12" s="8">
-        <v>43459</v>
-      </c>
-      <c r="D12" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B13" s="42"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B14" s="42"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B15" s="42"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B16" s="42"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="43"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C18" s="15"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C19" s="15"/>
+      <c r="B19" s="38">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C20" s="15"/>
+      <c r="B20" s="38">
+        <v>16</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B21" s="38">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B22" s="38">
+        <v>18</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B23" s="38">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B24" s="38"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B25" s="38"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B26" s="38"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B27" s="38"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B28" s="38"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B29" s="38"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B30" s="38"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B31" s="38"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="39"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C35" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1514,164 +1910,164 @@
   <dimension ref="B3:E32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="6.09765625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="6.19921875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.09765625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" style="13" customWidth="1"/>
     <col min="4" max="4" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C4" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="59">
+        <v>43456</v>
+      </c>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B8" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C9" s="13" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B4" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="44">
-        <v>43456</v>
-      </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B8" s="16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C9" s="16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C13" s="13" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C13" s="16" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B17" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B17" s="16" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C18" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C18" s="16" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C19" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C19" s="16" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C20" s="13" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C20" s="16" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B24" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B24" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C25" s="16" t="s">
-        <v>36</v>
+      <c r="C25" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C29" s="16" t="s">
-        <v>38</v>
+      <c r="C29" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="D31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="C32" s="16" t="s">
-        <v>42</v>
+      <c r="C32" s="13" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1687,10 +2083,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:S14"/>
+  <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1700,321 +2096,188 @@
     <col min="4" max="4" width="5.09765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="7.5" customWidth="1"/>
-    <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="41.09765625" customWidth="1"/>
-    <col min="12" max="12" width="6.19921875" customWidth="1"/>
+    <col min="7" max="9" width="7.5" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="41.09765625" customWidth="1"/>
+    <col min="13" max="13" width="6.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="16" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B2" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="L3" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="50" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="R3" s="46"/>
-      <c r="S3" s="47"/>
-    </row>
-    <row r="4" spans="2:19" s="17" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="37" t="s">
+      <c r="D5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B6" s="24">
+        <v>2</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="38" t="s">
+      <c r="F6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B7" s="24">
+        <v>3</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B8" s="24">
+        <v>4</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="L4" s="49"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B5" s="23">
-        <v>1</v>
-      </c>
-      <c r="C5" s="24" t="s">
+    </row>
+    <row r="9" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="26">
+        <v>5</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="23">
-        <v>1</v>
-      </c>
-      <c r="M5" s="24" t="s">
+      <c r="E9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="P5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="35"/>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B6" s="27">
-        <v>2</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J6" s="28"/>
-      <c r="L6" s="27">
-        <v>2</v>
-      </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21">
-        <v>38.33</v>
-      </c>
-      <c r="O6" s="21">
-        <v>38.26</v>
-      </c>
-      <c r="P6" s="21">
-        <v>4.03</v>
-      </c>
-      <c r="Q6" s="21">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="R6" s="21">
-        <v>40.6</v>
-      </c>
-      <c r="S6" s="28">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B7" s="27">
-        <v>3</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="28"/>
-      <c r="L7" s="27">
-        <v>3</v>
-      </c>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21">
-        <v>34.06</v>
-      </c>
-      <c r="O7" s="21">
-        <v>34.409999999999997</v>
-      </c>
-      <c r="P7" s="21">
-        <v>3.6280000000000001</v>
-      </c>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="28"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B8" s="27">
-        <v>4</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="27">
-        <v>4</v>
-      </c>
-      <c r="M8" s="21"/>
-      <c r="N8" s="56">
-        <v>49.42</v>
-      </c>
-      <c r="O8" s="56">
-        <v>49.4</v>
-      </c>
-      <c r="P8" s="21">
-        <v>3.97</v>
-      </c>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="28"/>
-    </row>
-    <row r="9" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="29">
-        <v>5</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J9" s="33"/>
-      <c r="L9" s="29">
-        <v>5</v>
-      </c>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32">
-        <v>37.94</v>
-      </c>
-      <c r="O9" s="32">
-        <v>38.15</v>
-      </c>
-      <c r="P9" s="32">
-        <v>3.96</v>
-      </c>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="33"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="L12" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="I13" s="18"/>
-      <c r="M13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="M14" t="s">
-        <v>63</v>
-      </c>
+      <c r="J9" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="J13" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2022,11 +2285,268 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC12502-9C27-4254-AB4E-CFA705610F51}">
-  <dimension ref="B4:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8599D64-2442-43DC-9DEE-9FA6DE56B094}">
+  <dimension ref="B3:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="3" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B4" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="K4" s="61"/>
+      <c r="L4" s="62"/>
+    </row>
+    <row r="5" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="64"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B6" s="20">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B7" s="24">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18">
+        <v>38.33</v>
+      </c>
+      <c r="E7" s="18">
+        <v>38.26</v>
+      </c>
+      <c r="F7" s="18">
+        <v>4.03</v>
+      </c>
+      <c r="G7" s="18">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="H7" s="18">
+        <v>40.6</v>
+      </c>
+      <c r="I7" s="25">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B8" s="24">
+        <v>3</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18">
+        <v>34.06</v>
+      </c>
+      <c r="E8" s="18">
+        <v>34.409999999999997</v>
+      </c>
+      <c r="F8" s="18">
+        <v>3.6280000000000001</v>
+      </c>
+      <c r="G8" s="18">
+        <v>32.1</v>
+      </c>
+      <c r="H8" s="18">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="I8" s="25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B9" s="24">
+        <v>4</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="44">
+        <v>49.42</v>
+      </c>
+      <c r="E9" s="44">
+        <v>49.4</v>
+      </c>
+      <c r="F9" s="18">
+        <v>3.97</v>
+      </c>
+      <c r="J9">
+        <v>20.25</v>
+      </c>
+      <c r="K9">
+        <v>20.3</v>
+      </c>
+      <c r="L9">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="26">
+        <v>5</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29">
+        <v>37.94</v>
+      </c>
+      <c r="E10" s="29">
+        <v>38.15</v>
+      </c>
+      <c r="F10" s="29">
+        <v>3.96</v>
+      </c>
+      <c r="J10">
+        <v>20.27</v>
+      </c>
+      <c r="K10">
+        <v>20.3</v>
+      </c>
+      <c r="L10">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="D11" s="67">
+        <v>34.4</v>
+      </c>
+      <c r="E11" s="67">
+        <v>34.5</v>
+      </c>
+      <c r="F11" s="67">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="D12" s="67">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E12" s="67">
+        <v>36</v>
+      </c>
+      <c r="F12" s="67">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B13" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="G16">
+        <v>20.25</v>
+      </c>
+      <c r="H16">
+        <v>20.3</v>
+      </c>
+      <c r="I16">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.4">
+      <c r="G17">
+        <v>20.27</v>
+      </c>
+      <c r="H17">
+        <v>20.3</v>
+      </c>
+      <c r="I17">
+        <v>1.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="J4:L4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC12502-9C27-4254-AB4E-CFA705610F51}">
+  <dimension ref="B4:P18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2034,77 +2554,188 @@
     <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>73</v>
       </c>
       <c r="C5">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="K5" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" t="s">
+        <v>104</v>
+      </c>
+      <c r="P5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6">
         <v>5.52</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="J6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6">
+        <v>0.25</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f>L6*M6</f>
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7">
         <v>7.48</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B10" s="57" t="s">
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K7">
+        <v>0.06</v>
+      </c>
+      <c r="L7">
+        <v>230</v>
+      </c>
+      <c r="M7">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <f>L7*M7</f>
+        <v>1610</v>
+      </c>
+      <c r="O7">
+        <f>O6*N7/N6</f>
+        <v>2576</v>
+      </c>
+      <c r="P7">
+        <v>12200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <v>0.27</v>
+      </c>
+      <c r="H8">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="G9">
+        <f>G7*G8</f>
+        <v>2.16</v>
+      </c>
+      <c r="H9">
+        <f>H7*H8</f>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B10" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
         <v>78</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>80</v>
       </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>88</v>
       </c>
       <c r="C15">
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16">
         <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>0.27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="C18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Pipette]Issue 및 ECO Update - SCH & PCB update 필요함.
</commit_message>
<xml_diff>
--- a/Plasma_Pipette_PP Issue list.xlsx
+++ b/Plasma_Pipette_PP Issue list.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FFBCB3-3BB8-45FE-B180-D26C67B04277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Issue" sheetId="1" r:id="rId1"/>
@@ -14,12 +13,12 @@
     <sheet name="Trans" sheetId="5" r:id="rId4"/>
     <sheet name="1225" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="120">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -479,13 +478,44 @@
   </si>
   <si>
     <t>완충 인식 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On시 Off됨.
+ - Power supply 사용시 정상 동작 : 2.3A 소모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery에서 Voltage drop 발생
+2A 이상 전류를 지원하는 Battery 필요
+Trans의 소모 전류 낮춤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Off시 On 상태를 그대로 유지하는 경우가 발생함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On후 board가 Reset되는 경우, S/V는 On 상태를 유지하고 있음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V에 current path 추가 - Diode 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEY_OP에 shunt Cap 4.7uF/25V 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="&quot;#&quot;00"/>
   </numFmts>
@@ -855,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1011,6 +1041,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1035,8 +1069,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1081,7 +1117,7 @@
         <xdr:cNvPr id="3" name="그림 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BA77CD3-E380-4C55-B6B7-B4FFD78D72CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BA77CD3-E380-4C55-B6B7-B4FFD78D72CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1131,7 +1167,7 @@
         <xdr:cNvPr id="5" name="그림 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0134AA55-8665-482A-BA8D-2E3884E21C46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0134AA55-8665-482A-BA8D-2E3884E21C46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1209,7 +1245,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1242,26 +1278,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1294,23 +1313,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1486,26 +1488,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.19921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.09765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="57.19921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.25" style="1" customWidth="1"/>
     <col min="7" max="7" width="59" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:7" s="5" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:7" s="5" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="54">
         <v>1</v>
       </c>
@@ -1545,7 +1547,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="38">
         <v>2</v>
       </c>
@@ -1563,7 +1565,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="38">
         <v>3</v>
       </c>
@@ -1581,7 +1583,7 @@
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B8" s="49">
         <v>4</v>
       </c>
@@ -1601,7 +1603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B9" s="49">
         <v>5</v>
       </c>
@@ -1621,7 +1623,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B10" s="40">
         <v>6</v>
       </c>
@@ -1641,7 +1643,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B11" s="40">
         <v>7</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B12" s="40">
         <v>8</v>
       </c>
@@ -1681,7 +1683,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="38">
         <v>9</v>
       </c>
@@ -1699,7 +1701,7 @@
       </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="2:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B14" s="38">
         <v>10</v>
       </c>
@@ -1715,11 +1717,11 @@
       <c r="F14" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="68" t="s">
+      <c r="G14" s="60" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="38">
         <v>11</v>
       </c>
@@ -1737,119 +1739,143 @@
       </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B16" s="38">
         <v>12</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C16" s="6">
+        <v>43470</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="38">
         <v>13</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="C17" s="6">
+        <v>43470</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="33" x14ac:dyDescent="0.3">
       <c r="B18" s="38">
         <v>14</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="F18" s="69" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="38">
         <v>15</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="69"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="38">
         <v>16</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="38">
         <v>17</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="38">
         <v>18</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="38">
         <v>19</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="69"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="38"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="69"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="38"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="69"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="38"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="38"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="38"/>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
@@ -1857,7 +1883,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="38"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
@@ -1865,7 +1891,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="38"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
@@ -1873,7 +1899,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="38"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
@@ -1881,7 +1907,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="39"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
@@ -1889,13 +1915,13 @@
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="12"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="12"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="12"/>
     </row>
   </sheetData>
@@ -1906,166 +1932,166 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.09765625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="6.19921875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="6.19921875" customWidth="1"/>
+    <col min="2" max="2" width="6.125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.25" style="13" customWidth="1"/>
+    <col min="4" max="4" width="6.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="61">
         <v>43456</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C9" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C12" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C13" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C18" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C19" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C20" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C25" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C29" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="13" t="s">
         <v>41</v>
       </c>
@@ -2082,33 +2108,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.796875" customWidth="1"/>
+    <col min="2" max="2" width="6.75" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="7.5" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="41.09765625" customWidth="1"/>
-    <col min="13" max="13" width="6.19921875" customWidth="1"/>
+    <col min="11" max="11" width="41.125" customWidth="1"/>
+    <col min="13" max="13" width="6.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="2:11" s="14" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:11" s="14" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="33" t="s">
         <v>42</v>
       </c>
@@ -2140,7 +2166,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="20">
         <v>1</v>
       </c>
@@ -2162,7 +2188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="24">
         <v>2</v>
       </c>
@@ -2188,7 +2214,7 @@
       </c>
       <c r="K6" s="25"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="24">
         <v>3</v>
       </c>
@@ -2216,7 +2242,7 @@
       </c>
       <c r="K7" s="25"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="24">
         <v>4</v>
       </c>
@@ -2246,7 +2272,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="26">
         <v>5</v>
       </c>
@@ -2274,7 +2300,7 @@
       </c>
       <c r="K9" s="30"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J13" s="15"/>
     </row>
   </sheetData>
@@ -2285,46 +2311,46 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8599D64-2442-43DC-9DEE-9FA6DE56B094}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B4" s="63" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61" t="s">
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="61" t="s">
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="62"/>
-    </row>
-    <row r="5" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="64"/>
-      <c r="C5" s="66"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="64"/>
+    </row>
+    <row r="5" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="66"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="36" t="s">
         <v>55</v>
       </c>
@@ -2353,7 +2379,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="20">
         <v>1</v>
       </c>
@@ -2373,7 +2399,7 @@
       <c r="H6" s="31"/>
       <c r="I6" s="32"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="24">
         <v>2</v>
       </c>
@@ -2397,7 +2423,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="24">
         <v>3</v>
       </c>
@@ -2421,7 +2447,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="24">
         <v>4</v>
       </c>
@@ -2445,7 +2471,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="26">
         <v>5</v>
       </c>
@@ -2469,44 +2495,44 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="D11" s="67">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D11" s="59">
         <v>34.4</v>
       </c>
-      <c r="E11" s="67">
+      <c r="E11" s="59">
         <v>34.5</v>
       </c>
-      <c r="F11" s="67">
+      <c r="F11" s="59">
         <v>3.3</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="D12" s="67">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="D12" s="59">
         <v>35.200000000000003</v>
       </c>
-      <c r="E12" s="67">
+      <c r="E12" s="59">
         <v>36</v>
       </c>
-      <c r="F12" s="67">
+      <c r="F12" s="59">
         <v>3.4</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G16">
         <v>20.25</v>
       </c>
@@ -2517,7 +2543,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G17">
         <v>20.27</v>
       </c>
@@ -2542,19 +2568,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC12502-9C27-4254-AB4E-CFA705610F51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -2565,7 +2591,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -2591,7 +2617,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -2621,7 +2647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>74</v>
       </c>
@@ -2658,7 +2684,7 @@
         <v>12200</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G8">
         <v>0.27</v>
       </c>
@@ -2666,7 +2692,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G9">
         <f>G7*G8</f>
         <v>2.16</v>
@@ -2676,7 +2702,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="45" t="s">
         <v>77</v>
       </c>
@@ -2684,7 +2710,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -2692,12 +2718,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>87</v>
       </c>
@@ -2705,7 +2731,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>88</v>
       </c>
@@ -2713,7 +2739,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>94</v>
       </c>
@@ -2724,7 +2750,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>0.14000000000000001</v>
       </c>

</xml_diff>